<commit_message>
Progressed through spring 2018 lure experiments
</commit_message>
<xml_diff>
--- a/output/y18-lures-cumulative.xlsx
+++ b/output/y18-lures-cumulative.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Charles.Burks\MyGit\ms-now-ppo-kairomone-2017-2yr\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A36DDD9F-2003-44C7-82F5-EEC3B70F6B9E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFED3F28-6156-4EF6-B940-B0D01D06FB1E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15468" yWindow="-108" windowWidth="15576" windowHeight="11904"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="y18-lures-cumulative" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Crop</t>
   </si>
@@ -104,12 +104,30 @@
   </si>
   <si>
     <t>Adults per trap per week</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>ab</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>bc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -643,7 +661,10 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -664,13 +685,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E16" totalsRowShown="0">
-  <tableColumns count="5">
-    <tableColumn id="1" name="Crop"/>
-    <tableColumn id="2" name="MD"/>
-    <tableColumn id="3" name="Treatment"/>
-    <tableColumn id="4" name="n" dataDxfId="1"/>
-    <tableColumn id="5" name="Adults per trap per week" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:F16" totalsRowShown="0">
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Crop"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="MD"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Treatment"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="n" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Adults per trap per week" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{0DAA8315-F4ED-4554-8C08-96DD8E4B7FAA}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -972,11 +994,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1001,6 +1023,9 @@
       <c r="E1" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1018,7 +1043,9 @@
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
@@ -1030,7 +1057,9 @@
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
@@ -1042,7 +1071,9 @@
       <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
@@ -1054,7 +1085,9 @@
       <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
@@ -1066,7 +1099,9 @@
       <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
@@ -1084,7 +1119,9 @@
       <c r="E7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
@@ -1096,7 +1133,9 @@
       <c r="E8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
@@ -1108,7 +1147,9 @@
       <c r="E9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
@@ -1120,7 +1161,9 @@
       <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
@@ -1132,7 +1175,9 @@
       <c r="E11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
@@ -1150,7 +1195,9 @@
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
@@ -1162,7 +1209,9 @@
       <c r="E13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
@@ -1174,7 +1223,9 @@
       <c r="E14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
@@ -1186,7 +1237,9 @@
       <c r="E15" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
@@ -1198,7 +1251,9 @@
       <c r="E16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>